<commit_message>
Commiting previous work before continuing
</commit_message>
<xml_diff>
--- a/app/tests/HMP1489_r1_t0.xlsx
+++ b/app/tests/HMP1489_r1_t0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -777,13 +777,13 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="2" sqref="E5 G21 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D6 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.5182186234818"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.1619433198381"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -915,7 +915,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1010,7 +1010,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1191,7 +1191,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1469,16 +1469,16 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="1" sqref="E5 G21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="1" sqref="D6 G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1831,16 +1831,16 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="2" sqref="E5 G21 B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
@@ -1953,10 +1953,10 @@
         <v>160</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>161</v>
@@ -2018,7 +2018,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D6 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2661,7 +2661,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2994,7 +2994,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3175,7 +3175,7 @@
   <dimension ref="A2:A12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3257,7 +3257,7 @@
   <dimension ref="A2:A19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3374,7 +3374,7 @@
   <dimension ref="A2:A19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3491,14 +3491,13 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="2" sqref="E5 G21 B15"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="D6 B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3645,7 +3644,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="77" zoomScaleNormal="77" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E5 G21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>